<commit_message>
Bug fix and more iterations
maximumstresslocal.m:
- fixed bug which placed the correct values in the wrong index of stressmaxlocal resulting in a failure to plot in an edge case

Iterations:
- slowly added stringers until I ran out of space on the spreadsheet
- followed direction of findpmax.m output (The maximum value of P is limited by the bottom/top surface) when adding additional stringers
- tried other positions along the way, used the most successful
- Progression:
  - 001
  - 002a
  - 002b
  - 003b
  - 004b
  - 005
  - 006
  - 007c
</commit_message>
<xml_diff>
--- a/src/Section Properties ITERATION002A.xlsx
+++ b/src/Section Properties ITERATION002A.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\A974V276\Documents\GitHub\structures-calc\src\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KMAC_PC\Documents\GitHub\structures-calc\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DAC316B-B1BD-4105-B3CB-F62E46B42352}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE9B3D2F-C2C1-4B32-AB9C-EAB12D7655CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-1500" yWindow="2520" windowWidth="30720" windowHeight="12828" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cross Section Properties" sheetId="1" r:id="rId1"/>
@@ -862,44 +862,44 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BB25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="12" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="25" max="26" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="16.7109375" customWidth="1"/>
-    <col min="30" max="30" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="33" max="35" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="36" max="37" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="25.7109375" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="25.7109375" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="25" max="26" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="16.6640625" customWidth="1"/>
+    <col min="30" max="30" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="33" max="35" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="36" max="37" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="25.5546875" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="25.5546875" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="25.33203125" bestFit="1" customWidth="1"/>
     <col min="49" max="49" width="25" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="23.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1036,7 +1036,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -1076,23 +1076,23 @@
       </c>
       <c r="K2">
         <f t="shared" ref="K2:K15" si="0">D2-$AH$3</f>
-        <v>0.52427118018903573</v>
+        <v>0.59222976068920719</v>
       </c>
       <c r="L2">
         <f t="shared" ref="L2:L15" si="1">E2-$AI$3</f>
-        <v>-0.34587660080488614</v>
+        <v>-0.34261305091703931</v>
       </c>
       <c r="M2">
         <f>C2*K2^2</f>
-        <v>6.4420375869563534E-2</v>
+        <v>8.2203770963905215E-2</v>
       </c>
       <c r="N2">
         <f>C2*L2^2</f>
-        <v>2.8038427261955289E-2</v>
+        <v>2.7511805310628541E-2</v>
       </c>
       <c r="O2">
         <f>C2*K2*L2</f>
-        <v>-4.2499953211816321E-2</v>
+        <v>-4.7556010582874376E-2</v>
       </c>
       <c r="P2">
         <v>255</v>
@@ -1115,23 +1115,23 @@
       </c>
       <c r="U2">
         <f t="shared" ref="U2:U15" si="3">D2-$AH$5</f>
-        <v>0.34307972631149136</v>
+        <v>0.66339223378477385</v>
       </c>
       <c r="V2">
         <f t="shared" ref="V2:V15" si="4">E2-$AI$5</f>
-        <v>-0.38941597600005751</v>
+        <v>-0.37403372639821697</v>
       </c>
       <c r="W2">
         <f>C2*U2^2</f>
-        <v>2.7586804360773706E-2</v>
+        <v>0.10314591933889501</v>
       </c>
       <c r="X2">
         <f>C2*V2^2</f>
-        <v>3.5541750554080632E-2</v>
+        <v>3.2789350425781925E-2</v>
       </c>
       <c r="Y2">
         <f>C2*U2*V2</f>
-        <v>-3.1312670265802034E-2</v>
+        <v>-5.8155719359255328E-2</v>
       </c>
       <c r="Z2">
         <v>1.47</v>
@@ -1190,7 +1190,7 @@
       </c>
       <c r="AT2">
         <f>-AI3</f>
-        <v>1.5291233991951139</v>
+        <v>1.5323869490829607</v>
       </c>
       <c r="AU2" t="s">
         <v>62</v>
@@ -1206,18 +1206,18 @@
       </c>
       <c r="AZ2">
         <f>(Q2)*(H2+X2)</f>
-        <v>3.9550494094082782E-2</v>
+        <v>3.9199563077724695E-2</v>
       </c>
       <c r="BA2">
         <f>(Q2)*(I2+W2)</f>
-        <v>3.5270450340259911E-3</v>
+        <v>1.3160832193736458E-2</v>
       </c>
       <c r="BB2">
         <f>(Q2)*(J2+Y2)</f>
-        <v>-3.992365458889759E-3</v>
+        <v>-7.4148542183050548E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -1258,23 +1258,23 @@
       </c>
       <c r="K3">
         <f t="shared" si="0"/>
-        <v>-0.50697881981096427</v>
+        <v>-0.43902023931079281</v>
       </c>
       <c r="L3">
         <f t="shared" si="1"/>
-        <v>-0.34587660080488614</v>
+        <v>-0.34261305091703931</v>
       </c>
       <c r="M3">
         <f t="shared" ref="M3:M15" si="7">C3*K3^2</f>
-        <v>6.2345940316234964E-2</v>
+        <v>4.6751724130700008E-2</v>
       </c>
       <c r="N3">
         <f t="shared" ref="N3:N15" si="8">C3*L3^2</f>
-        <v>2.9018229534864898E-2</v>
+        <v>2.8473204790112783E-2</v>
       </c>
       <c r="O3">
         <f t="shared" ref="O3:O15" si="9">C3*K3*L3</f>
-        <v>4.2534325040647983E-2</v>
+        <v>3.6485221877690134E-2</v>
       </c>
       <c r="P3">
         <v>255</v>
@@ -1297,23 +1297,23 @@
       </c>
       <c r="U3">
         <f t="shared" si="3"/>
-        <v>-0.68817027368850869</v>
+        <v>-0.36785776621522615</v>
       </c>
       <c r="V3">
         <f t="shared" si="4"/>
-        <v>-0.38941597600005751</v>
+        <v>-0.37403372639821697</v>
       </c>
       <c r="W3">
         <f t="shared" ref="W3:W15" si="13">C3*U3^2</f>
-        <v>0.11487363529372573</v>
+        <v>3.2823765850080643E-2</v>
       </c>
       <c r="X3">
         <f t="shared" ref="X3:X15" si="14">C3*V3^2</f>
-        <v>3.6783756307496286E-2</v>
+        <v>3.3935173612448445E-2</v>
       </c>
       <c r="Y3">
         <f t="shared" ref="Y3:Y15" si="15">C3*U3*V3</f>
-        <v>6.5003721484239732E-2</v>
+        <v>3.3374843711047444E-2</v>
       </c>
       <c r="Z3">
         <v>1.47</v>
@@ -1339,27 +1339,27 @@
       </c>
       <c r="AH3">
         <f>F16/C16</f>
-        <v>-0.49302118018903573</v>
+        <v>-0.56097976068920719</v>
       </c>
       <c r="AI3">
         <f>G16/C16</f>
-        <v>-1.5291233991951139</v>
+        <v>-1.5323869490829607</v>
       </c>
       <c r="AJ3">
         <f>H16+N16</f>
-        <v>1.0864018626510268</v>
+        <v>1.0790555408169558</v>
       </c>
       <c r="AK3">
         <f>I16+M16</f>
-        <v>0.52203122573857619</v>
+        <v>0.46781680918671636</v>
       </c>
       <c r="AL3">
         <f>J16+O16</f>
-        <v>-0.12652458320020382</v>
+        <v>-0.20431446464994504</v>
       </c>
       <c r="AM3">
         <f>(AJ3*AK3)-AL3^2</f>
-        <v>0.55112722585040252</v>
+        <v>0.46305591957504116</v>
       </c>
       <c r="AO3" t="s">
         <v>62</v>
@@ -1378,7 +1378,7 @@
       </c>
       <c r="AT3">
         <f>-1.875-AI3</f>
-        <v>-0.34587660080488614</v>
+        <v>-0.34261305091703931</v>
       </c>
       <c r="AU3" t="s">
         <v>62</v>
@@ -1394,18 +1394,18 @@
       </c>
       <c r="AZ3">
         <f t="shared" ref="AZ3:AZ15" si="17">(Q3)*(H3+X3)</f>
-        <v>7.2765835231587937E-3</v>
+        <v>6.913389229540194E-3</v>
       </c>
       <c r="BA3">
         <f t="shared" ref="BA3:BA15" si="18">(Q3)*(I3+W3)</f>
-        <v>5.0889713255479502E-2</v>
+        <v>4.0428354901414748E-2</v>
       </c>
       <c r="BB3">
         <f t="shared" ref="BB3:BB15" si="19">(Q3)*(J3+Y3)</f>
-        <v>-1.3742274710206144E-3</v>
+        <v>-5.4069093871026309E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -1445,23 +1445,23 @@
       </c>
       <c r="K4">
         <f t="shared" si="0"/>
-        <v>-0.25697881981096427</v>
+        <v>-0.18902023931079281</v>
       </c>
       <c r="L4">
         <f t="shared" si="1"/>
-        <v>1.4666233991951139</v>
+        <v>1.4698869490829607</v>
       </c>
       <c r="M4">
         <f t="shared" si="7"/>
-        <v>1.2382146343394258E-2</v>
+        <v>6.6991220379580092E-3</v>
       </c>
       <c r="N4">
         <f t="shared" si="8"/>
-        <v>0.40330953657499313</v>
+        <v>0.40510643307832761</v>
       </c>
       <c r="O4">
         <f t="shared" si="9"/>
-        <v>-7.0667090668557198E-2</v>
+        <v>-5.2094696789151067E-2</v>
       </c>
       <c r="P4">
         <v>155</v>
@@ -1484,23 +1484,23 @@
       </c>
       <c r="U4">
         <f t="shared" si="3"/>
-        <v>-0.43817027368850864</v>
+        <v>-0.11785776621522615</v>
       </c>
       <c r="V4">
         <f t="shared" si="4"/>
-        <v>1.4230840239999425</v>
+        <v>1.438466273601783</v>
       </c>
       <c r="W4">
         <f t="shared" si="13"/>
-        <v>3.5998722889549237E-2</v>
+        <v>2.6044599482330441E-3</v>
       </c>
       <c r="X4">
         <f t="shared" si="14"/>
-        <v>0.37971902613072539</v>
+        <v>0.38797222880433746</v>
       </c>
       <c r="Y4">
         <f t="shared" si="15"/>
-        <v>-0.11691620930208731</v>
+        <v>-3.1787704084246214E-2</v>
       </c>
       <c r="Z4">
         <v>0.63</v>
@@ -1575,18 +1575,18 @@
       </c>
       <c r="AZ4">
         <f t="shared" si="17"/>
-        <v>2.9447145423568716E-2</v>
+        <v>3.0086768630773652E-2</v>
       </c>
       <c r="BA4">
         <f t="shared" si="18"/>
-        <v>4.6063072739400655E-3</v>
+        <v>2.0182518959880611E-3</v>
       </c>
       <c r="BB4">
         <f t="shared" si="19"/>
-        <v>-9.0610062209117662E-3</v>
+        <v>-2.4635470665290817E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -1626,23 +1626,23 @@
       </c>
       <c r="K5">
         <f t="shared" si="0"/>
-        <v>0.24302118018903573</v>
+        <v>0.31097976068920719</v>
       </c>
       <c r="L5">
         <f t="shared" si="1"/>
-        <v>-2.1583766008048864</v>
+        <v>-2.1551130509170395</v>
       </c>
       <c r="M5">
         <f t="shared" si="7"/>
-        <v>3.691205876279486E-3</v>
+        <v>6.0442757223947855E-3</v>
       </c>
       <c r="N5">
         <f t="shared" si="8"/>
-        <v>0.29116184693137848</v>
+        <v>0.29028201638955942</v>
       </c>
       <c r="O5">
         <f t="shared" si="9"/>
-        <v>-3.2783201801250168E-2</v>
+        <v>-4.1887283802023008E-2</v>
       </c>
       <c r="P5">
         <v>155</v>
@@ -1665,23 +1665,23 @@
       </c>
       <c r="U5">
         <f t="shared" si="3"/>
-        <v>6.1829726311491362E-2</v>
+        <v>0.38214223378477385</v>
       </c>
       <c r="V5">
         <f t="shared" si="4"/>
-        <v>-2.2019159760000573</v>
+        <v>-2.186533726398217</v>
       </c>
       <c r="W5">
         <f t="shared" si="13"/>
-        <v>2.3893219098462045E-4</v>
+        <v>9.1270429276260473E-3</v>
       </c>
       <c r="X5">
         <f t="shared" si="14"/>
-        <v>0.30302712283526778</v>
+        <v>0.29880810854230455</v>
       </c>
       <c r="Y5">
         <f t="shared" si="15"/>
-        <v>-8.5089913848114956E-3</v>
+        <v>-5.2222930153222512E-2</v>
       </c>
       <c r="Z5">
         <v>0.63</v>
@@ -1707,27 +1707,27 @@
       </c>
       <c r="AH5">
         <f>S16/R16</f>
-        <v>-0.31182972631149136</v>
+        <v>-0.63214223378477385</v>
       </c>
       <c r="AI5">
         <f>T16/R16</f>
-        <v>-1.4855840239999425</v>
+        <v>-1.500966273601783</v>
       </c>
       <c r="AJ5">
         <f>AZ16</f>
-        <v>0.12093379482690673</v>
+        <v>0.11688575980995447</v>
       </c>
       <c r="AK5">
         <f>BA16</f>
-        <v>9.2271017418334988E-2</v>
+        <v>6.4777016011741073E-2</v>
       </c>
       <c r="AL5">
         <f>BB16</f>
-        <v>1.1382984695428649E-2</v>
+        <v>-3.1424341689118264E-2</v>
       </c>
       <c r="AM5">
         <f>(AJ5*AK5)-AL5^2</f>
-        <v>1.1029111948362497E-2</v>
+        <v>6.5840214841594857E-3</v>
       </c>
       <c r="AO5" t="s">
         <v>62</v>
@@ -1758,18 +1758,18 @@
       </c>
       <c r="AZ5">
         <f t="shared" si="17"/>
-        <v>2.3490908985879085E-2</v>
+        <v>2.3163935378174433E-2</v>
       </c>
       <c r="BA5">
         <f t="shared" si="18"/>
-        <v>1.1942870313464142E-4</v>
+        <v>8.08257285224352E-4</v>
       </c>
       <c r="BB5">
         <f t="shared" si="19"/>
-        <v>-6.5944683232289089E-4</v>
+        <v>-4.0472770868747445E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -1808,7 +1808,7 @@
       </c>
       <c r="K6">
         <f t="shared" si="0"/>
-        <v>0.61802118018903573</v>
+        <v>0.68597976068920719</v>
       </c>
       <c r="L6" t="e">
         <f t="shared" si="1"/>
@@ -1816,7 +1816,7 @@
       </c>
       <c r="M6">
         <f t="shared" si="7"/>
-        <v>5.9679715494101336E-3</v>
+        <v>7.3526286261753433E-3</v>
       </c>
       <c r="N6" t="e">
         <f t="shared" si="8"/>
@@ -1847,7 +1847,7 @@
       </c>
       <c r="U6">
         <f t="shared" si="3"/>
-        <v>0.43682972631149136</v>
+        <v>0.75714223378477385</v>
       </c>
       <c r="V6" t="e">
         <f t="shared" si="4"/>
@@ -1855,7 +1855,7 @@
       </c>
       <c r="W6">
         <f t="shared" si="13"/>
-        <v>2.9815657779589445E-3</v>
+        <v>8.9572556590718309E-3</v>
       </c>
       <c r="X6" t="e">
         <f t="shared" si="14"/>
@@ -1923,14 +1923,14 @@
       </c>
       <c r="BA6">
         <f t="shared" si="18"/>
-        <v>1.696079618973887E-3</v>
+        <v>5.0723444018026679E-3</v>
       </c>
       <c r="BB6" t="e">
         <f t="shared" si="19"/>
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="7" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -1969,7 +1969,7 @@
       </c>
       <c r="K7">
         <f t="shared" si="0"/>
-        <v>0.61802118018903573</v>
+        <v>0.68597976068920719</v>
       </c>
       <c r="L7" t="e">
         <f t="shared" si="1"/>
@@ -1977,7 +1977,7 @@
       </c>
       <c r="M7">
         <f t="shared" si="7"/>
-        <v>5.9679715494101336E-3</v>
+        <v>7.3526286261753433E-3</v>
       </c>
       <c r="N7" t="e">
         <f t="shared" si="8"/>
@@ -2008,7 +2008,7 @@
       </c>
       <c r="U7">
         <f t="shared" si="3"/>
-        <v>0.43682972631149136</v>
+        <v>0.75714223378477385</v>
       </c>
       <c r="V7" t="e">
         <f t="shared" si="4"/>
@@ -2016,7 +2016,7 @@
       </c>
       <c r="W7">
         <f t="shared" si="13"/>
-        <v>2.9815657779589445E-3</v>
+        <v>8.9572556590718309E-3</v>
       </c>
       <c r="X7" t="e">
         <f t="shared" si="14"/>
@@ -2084,14 +2084,14 @@
       </c>
       <c r="BA7">
         <f t="shared" si="18"/>
-        <v>1.696079618973887E-3</v>
+        <v>5.0723444018026679E-3</v>
       </c>
       <c r="BB7" t="e">
         <f t="shared" si="19"/>
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="8" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -2130,7 +2130,7 @@
       </c>
       <c r="K8">
         <f t="shared" si="0"/>
-        <v>0.61802118018903573</v>
+        <v>0.68597976068920719</v>
       </c>
       <c r="L8" t="e">
         <f t="shared" si="1"/>
@@ -2138,7 +2138,7 @@
       </c>
       <c r="M8">
         <f t="shared" si="7"/>
-        <v>5.9679715494101336E-3</v>
+        <v>7.3526286261753433E-3</v>
       </c>
       <c r="N8" t="e">
         <f t="shared" si="8"/>
@@ -2169,7 +2169,7 @@
       </c>
       <c r="U8">
         <f t="shared" si="3"/>
-        <v>0.43682972631149136</v>
+        <v>0.75714223378477385</v>
       </c>
       <c r="V8" t="e">
         <f t="shared" si="4"/>
@@ -2177,7 +2177,7 @@
       </c>
       <c r="W8">
         <f t="shared" si="13"/>
-        <v>2.9815657779589445E-3</v>
+        <v>8.9572556590718309E-3</v>
       </c>
       <c r="X8" t="e">
         <f t="shared" si="14"/>
@@ -2250,14 +2250,14 @@
       </c>
       <c r="BA8">
         <f t="shared" si="18"/>
-        <v>1.696079618973887E-3</v>
+        <v>5.0723444018026679E-3</v>
       </c>
       <c r="BB8" t="e">
         <f t="shared" si="19"/>
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="9" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -2296,7 +2296,7 @@
       </c>
       <c r="K9">
         <f t="shared" si="0"/>
-        <v>0.61802118018903573</v>
+        <v>0.68597976068920719</v>
       </c>
       <c r="L9" t="e">
         <f t="shared" si="1"/>
@@ -2304,7 +2304,7 @@
       </c>
       <c r="M9">
         <f t="shared" si="7"/>
-        <v>5.9679715494101336E-3</v>
+        <v>7.3526286261753433E-3</v>
       </c>
       <c r="N9" t="e">
         <f t="shared" si="8"/>
@@ -2335,7 +2335,7 @@
       </c>
       <c r="U9">
         <f t="shared" si="3"/>
-        <v>0.43682972631149136</v>
+        <v>0.75714223378477385</v>
       </c>
       <c r="V9" t="e">
         <f t="shared" si="4"/>
@@ -2343,7 +2343,7 @@
       </c>
       <c r="W9">
         <f t="shared" si="13"/>
-        <v>2.9815657779589445E-3</v>
+        <v>8.9572556590718309E-3</v>
       </c>
       <c r="X9" t="e">
         <f t="shared" si="14"/>
@@ -2420,14 +2420,14 @@
       </c>
       <c r="BA9">
         <f t="shared" si="18"/>
-        <v>1.696079618973887E-3</v>
+        <v>5.0723444018026679E-3</v>
       </c>
       <c r="BB9" t="e">
         <f t="shared" si="19"/>
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="10" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -2466,7 +2466,7 @@
       </c>
       <c r="K10">
         <f t="shared" si="0"/>
-        <v>0.61802118018903573</v>
+        <v>0.68597976068920719</v>
       </c>
       <c r="L10" t="e">
         <f t="shared" si="1"/>
@@ -2474,7 +2474,7 @@
       </c>
       <c r="M10">
         <f t="shared" si="7"/>
-        <v>5.9679715494101336E-3</v>
+        <v>7.3526286261753433E-3</v>
       </c>
       <c r="N10" t="e">
         <f t="shared" si="8"/>
@@ -2505,7 +2505,7 @@
       </c>
       <c r="U10">
         <f t="shared" si="3"/>
-        <v>0.43682972631149136</v>
+        <v>0.75714223378477385</v>
       </c>
       <c r="V10" t="e">
         <f t="shared" si="4"/>
@@ -2513,7 +2513,7 @@
       </c>
       <c r="W10">
         <f t="shared" si="13"/>
-        <v>2.9815657779589445E-3</v>
+        <v>8.9572556590718309E-3</v>
       </c>
       <c r="X10" t="e">
         <f t="shared" si="14"/>
@@ -2592,14 +2592,14 @@
       </c>
       <c r="BA10">
         <f t="shared" si="18"/>
-        <v>1.696079618973887E-3</v>
+        <v>5.0723444018026679E-3</v>
       </c>
       <c r="BB10" t="e">
         <f t="shared" si="19"/>
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="11" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -2611,19 +2611,20 @@
         <v>1.5625E-2</v>
       </c>
       <c r="D11" s="5">
-        <v>1.625</v>
+        <f>-1.6046754518</f>
+        <v>-1.6046754517999999</v>
       </c>
       <c r="E11" s="5">
-        <f>0.5*(1/8)</f>
-        <v>6.25E-2</v>
+        <f>-0.092597515</f>
+        <v>-9.2597515000000005E-2</v>
       </c>
       <c r="F11">
         <f t="shared" si="5"/>
-        <v>2.5390625E-2</v>
+        <v>-2.5073053934374999E-2</v>
       </c>
       <c r="G11">
         <f t="shared" si="6"/>
-        <v>9.765625E-4</v>
+        <v>-1.4468361718750001E-3</v>
       </c>
       <c r="H11">
         <f t="shared" si="22"/>
@@ -2638,23 +2639,23 @@
       </c>
       <c r="K11">
         <f t="shared" si="0"/>
-        <v>2.1180211801890358</v>
+        <v>-1.0436956911107926</v>
       </c>
       <c r="L11">
         <f t="shared" si="1"/>
-        <v>1.5916233991951139</v>
+        <v>1.4397894340829607</v>
       </c>
       <c r="M11">
         <f>C11*K11^2</f>
-        <v>7.0093964370771186E-2</v>
+        <v>1.702032336942555E-2</v>
       </c>
       <c r="N11">
         <f t="shared" si="8"/>
-        <v>3.9582266326022013E-2</v>
+        <v>3.2390525226514567E-2</v>
       </c>
       <c r="O11">
         <f t="shared" si="9"/>
-        <v>5.2673313599683122E-2</v>
+        <v>-2.3479719194675511E-2</v>
       </c>
       <c r="P11">
         <v>1130</v>
@@ -2669,31 +2670,31 @@
       </c>
       <c r="S11">
         <f t="shared" si="11"/>
-        <v>1.4345703124999998E-2</v>
+        <v>-1.4166275472921873E-2</v>
       </c>
       <c r="T11">
         <f t="shared" si="12"/>
-        <v>5.5175781249999995E-4</v>
+        <v>-8.1746243710937498E-4</v>
       </c>
       <c r="U11">
         <f t="shared" si="3"/>
-        <v>1.9368297263114913</v>
+        <v>-0.97253321801522608</v>
       </c>
       <c r="V11">
         <f t="shared" si="4"/>
-        <v>1.5480840239999425</v>
+        <v>1.408368758601783</v>
       </c>
       <c r="W11">
         <f t="shared" si="13"/>
-        <v>5.8614209198810101E-2</v>
+        <v>1.4778450939735175E-2</v>
       </c>
       <c r="X11">
         <f t="shared" si="14"/>
-        <v>3.7446314771310225E-2</v>
+        <v>3.0992227503211366E-2</v>
       </c>
       <c r="Y11">
         <f t="shared" si="15"/>
-        <v>4.6849611820484388E-2</v>
+        <v>-2.1401334389923456E-2</v>
       </c>
       <c r="Z11">
         <v>7.8</v>
@@ -2758,18 +2759,18 @@
       </c>
       <c r="AZ11">
         <f t="shared" si="17"/>
-        <v>2.1168662800217359E-2</v>
+        <v>1.7522103493741503E-2</v>
       </c>
       <c r="BA11">
         <f t="shared" si="18"/>
-        <v>3.3128523151754789E-2</v>
+        <v>8.3613197353774576E-3</v>
       </c>
       <c r="BB11">
         <f t="shared" si="19"/>
-        <v>2.6470030678573678E-2</v>
+        <v>-1.2091753930306752E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -2940,7 +2941,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="13" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -3097,7 +3098,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="14" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -3254,7 +3255,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="15" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>25</v>
       </c>
@@ -3411,7 +3412,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="16" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>32</v>
       </c>
@@ -3421,11 +3422,11 @@
       </c>
       <c r="F16" s="2">
         <f>SUM(F2:F5,F11)</f>
-        <v>-0.36610038587906291</v>
+        <v>-0.41656406481343788</v>
       </c>
       <c r="G16" s="2">
         <f t="shared" ref="G16:J16" si="23">SUM(G2:G5,G11)</f>
-        <v>-1.1354738680544929</v>
+        <v>-1.1378972667263678</v>
       </c>
       <c r="H16" s="2">
         <f t="shared" si="23"/>
@@ -3441,15 +3442,15 @@
       </c>
       <c r="M16" s="2">
         <f>SUM(M2:M5,M11)</f>
-        <v>0.21293363277624344</v>
+        <v>0.15871921622438356</v>
       </c>
       <c r="N16" s="2">
         <f t="shared" ref="N16:O16" si="24">SUM(N2:N5,N11)</f>
-        <v>0.79111030662921389</v>
+        <v>0.78376398479514287</v>
       </c>
       <c r="O16" s="2">
         <f t="shared" si="24"/>
-        <v>-5.0742607041292589E-2</v>
+        <v>-0.12853248849103383</v>
       </c>
       <c r="R16" s="2">
         <f>SUM(R2:R5,R11)</f>
@@ -3457,38 +3458,38 @@
       </c>
       <c r="S16" s="2">
         <f t="shared" ref="S16:T16" si="25">SUM(S2:S5,S11)</f>
-        <v>-2.7756900762080518E-2</v>
+        <v>-5.626887936000239E-2</v>
       </c>
       <c r="T16" s="2">
         <f t="shared" si="25"/>
-        <v>-0.13223629708319784</v>
+        <v>-0.13360551733280721</v>
       </c>
       <c r="W16" s="2">
         <f>SUM(W2:W5,W11)</f>
-        <v>0.23731230393384337</v>
+        <v>0.16247963900456991</v>
       </c>
       <c r="X16" s="2">
         <f t="shared" ref="X16:Y16" si="26">SUM(X2:X5,X11)</f>
-        <v>0.79251797059888029</v>
+        <v>0.78449708888808378</v>
       </c>
       <c r="Y16" s="2">
         <f t="shared" si="26"/>
-        <v>-4.4884537647976716E-2</v>
+        <v>-0.13019284427560007</v>
       </c>
       <c r="AZ16" s="2">
         <f>SUM(AZ2:AZ5,AZ11)</f>
-        <v>0.12093379482690673</v>
+        <v>0.11688575980995447</v>
       </c>
       <c r="BA16" s="2">
         <f t="shared" ref="BA16:BB16" si="27">SUM(BA2:BA5,BA11)</f>
-        <v>9.2271017418334988E-2</v>
+        <v>6.4777016011741073E-2</v>
       </c>
       <c r="BB16" s="2">
         <f t="shared" si="27"/>
-        <v>1.1382984695428649E-2</v>
+        <v>-3.1424341689118264E-2</v>
       </c>
     </row>
-    <row r="21" spans="17:22" x14ac:dyDescent="0.25">
+    <row r="21" spans="17:22" x14ac:dyDescent="0.3">
       <c r="Q21" s="1"/>
       <c r="R21" s="4" t="s">
         <v>54</v>
@@ -3496,13 +3497,13 @@
       <c r="S21" s="4"/>
       <c r="T21" s="4"/>
     </row>
-    <row r="22" spans="17:22" x14ac:dyDescent="0.25">
+    <row r="22" spans="17:22" x14ac:dyDescent="0.3">
       <c r="Q22" s="2"/>
       <c r="R22" s="3" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="23" spans="17:22" x14ac:dyDescent="0.25">
+    <row r="23" spans="17:22" x14ac:dyDescent="0.3">
       <c r="Q23" s="6" t="s">
         <v>36</v>
       </c>
@@ -3512,7 +3513,7 @@
       <c r="U23" s="6"/>
       <c r="V23" s="6"/>
     </row>
-    <row r="24" spans="17:22" x14ac:dyDescent="0.25">
+    <row r="24" spans="17:22" x14ac:dyDescent="0.3">
       <c r="Q24" s="6"/>
       <c r="R24" s="6"/>
       <c r="S24" s="6"/>
@@ -3520,7 +3521,7 @@
       <c r="U24" s="6"/>
       <c r="V24" s="6"/>
     </row>
-    <row r="25" spans="17:22" x14ac:dyDescent="0.25">
+    <row r="25" spans="17:22" x14ac:dyDescent="0.3">
       <c r="Q25" s="6"/>
       <c r="R25" s="6"/>
       <c r="S25" s="6"/>

</xml_diff>